<commit_message>
Finalized the system completely.
</commit_message>
<xml_diff>
--- a/data/cashflow_data/plus91_share_transfers.xlsx
+++ b/data/cashflow_data/plus91_share_transfers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t xml:space="preserve">broker_code</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">JC555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ081</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -189,6 +192,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -383,10 +394,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -602,6 +613,19 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>45608</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>1770000</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>